<commit_message>
Finished updating figures to use Helvetica for PLOS and final check-through of edits
</commit_message>
<xml_diff>
--- a/draft/plos/fig2/heatmap.xlsx
+++ b/draft/plos/fig2/heatmap.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="0" windowWidth="33740" windowHeight="21140" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28320" windowHeight="16920" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -697,7 +697,7 @@
     <numFmt numFmtId="164" formatCode=";;;"/>
     <numFmt numFmtId="165" formatCode=";;"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -766,15 +766,24 @@
       <name val="Helvetica"/>
     </font>
     <font>
+      <sz val="144"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b/>
       <sz val="95"/>
       <color theme="1"/>
-      <name val="Myriad Pro"/>
-    </font>
-    <font>
-      <sz val="144"/>
-      <color theme="1"/>
-      <name val="Myriad Pro"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="2">
@@ -850,7 +859,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -872,12 +881,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -996,7 +1007,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1550,11 +1560,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2090604952"/>
-        <c:axId val="2090607912"/>
+        <c:axId val="2109784328"/>
+        <c:axId val="2109781368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2090604952"/>
+        <c:axId val="2109784328"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1565,12 +1575,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090607912"/>
+        <c:crossAx val="2109781368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2090607912"/>
+        <c:axId val="2109781368"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1582,14 +1592,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090604952"/>
+        <c:crossAx val="2109784328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3967,7 +3976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
@@ -8117,8 +8126,8 @@
   </sheetPr>
   <dimension ref="B1:Y104"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A77" zoomScale="16" zoomScaleNormal="16" zoomScalePageLayoutView="16" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="15" zoomScaleNormal="15" zoomScalePageLayoutView="15" workbookViewId="0">
+      <selection activeCell="AB77" sqref="AB77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="180" customHeight="1" x14ac:dyDescent="0"/>
@@ -8127,10 +8136,10 @@
     <col min="2" max="2" width="30" style="13" customWidth="1"/>
     <col min="3" max="5" width="30" style="6" customWidth="1"/>
     <col min="6" max="6" width="1.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="15"/>
-    <col min="8" max="8" width="69.6640625" style="16" customWidth="1"/>
-    <col min="9" max="9" width="27.33203125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="82.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="69.6640625" style="15" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" style="16" customWidth="1"/>
+    <col min="10" max="10" width="129.33203125" style="16" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
@@ -8153,13 +8162,13 @@
       <c r="E2" s="6">
         <v>-0.64594642082365272</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="6">
-        <v>1</v>
-      </c>
-      <c r="J2" s="14">
+      <c r="I2" s="17">
+        <v>1</v>
+      </c>
+      <c r="J2" s="18">
         <v>1</v>
       </c>
       <c r="L2" s="4"/>
@@ -8179,13 +8188,13 @@
       <c r="E3" s="6">
         <v>-1.1932511226035434</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="17">
         <v>0.5</v>
       </c>
-      <c r="J3" s="14"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" spans="2:25" ht="180" customHeight="1">
       <c r="B4" s="11">
@@ -8200,13 +8209,13 @@
       <c r="E4" s="6">
         <v>-0.29229837696333849</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="17">
         <v>0.25</v>
       </c>
-      <c r="J4" s="14"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="2:25" ht="180" customHeight="1">
       <c r="B5" s="11">
@@ -8221,13 +8230,13 @@
       <c r="E5" s="6">
         <v>-0.57341814749162889</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="17">
         <v>0</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="18">
         <v>0</v>
       </c>
     </row>
@@ -8244,13 +8253,13 @@
       <c r="E6" s="6">
         <v>-1.4384859308548541</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="17">
         <v>-1.25</v>
       </c>
-      <c r="J6" s="14"/>
+      <c r="J6" s="18"/>
     </row>
     <row r="7" spans="2:25" ht="180" customHeight="1">
       <c r="B7" s="11">
@@ -8261,13 +8270,13 @@
       <c r="E7" s="6">
         <v>-4.7575225530421061</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="17">
         <v>-2.5</v>
       </c>
-      <c r="J7" s="14"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="2:25" ht="180" customHeight="1">
       <c r="B8" s="11">
@@ -8278,13 +8287,13 @@
       <c r="E8" s="6">
         <v>-4.331553820769825</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="17">
         <v>-5</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="18">
         <v>-5</v>
       </c>
       <c r="K8" s="9"/>
@@ -8301,7 +8310,7 @@
       <c r="E9" s="6">
         <v>-4.53567380342575</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="14" t="s">
         <v>121</v>
       </c>
       <c r="K9" s="9"/>
@@ -8316,7 +8325,7 @@
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>122</v>
       </c>
       <c r="K10" s="9"/>
@@ -8337,7 +8346,7 @@
       <c r="E11" s="6">
         <v>-0.31413959689263216</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="14" t="s">
         <v>123</v>
       </c>
       <c r="K11" s="9"/>
@@ -8358,7 +8367,7 @@
       <c r="E12" s="6">
         <v>-0.18516993693403894</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="14" t="s">
         <v>124</v>
       </c>
       <c r="Y12" s="5" t="s">
@@ -8372,7 +8381,7 @@
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="14" t="s">
         <v>125</v>
       </c>
     </row>
@@ -8389,7 +8398,7 @@
       <c r="E14" s="6">
         <v>-0.13399760761628876</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>126</v>
       </c>
     </row>
@@ -8406,7 +8415,7 @@
       <c r="E15" s="6">
         <v>-0.23464380776176874</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="14" t="s">
         <v>127</v>
       </c>
     </row>
@@ -8423,7 +8432,7 @@
       <c r="E16" s="6">
         <v>-3.320829955378052</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="14" t="s">
         <v>128</v>
       </c>
     </row>
@@ -8440,7 +8449,7 @@
       <c r="E17" s="6">
         <v>-1.2582938287584953</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="14" t="s">
         <v>129</v>
       </c>
     </row>
@@ -8451,7 +8460,7 @@
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="14" t="s">
         <v>130</v>
       </c>
     </row>
@@ -8468,7 +8477,7 @@
       <c r="E19" s="6">
         <v>-2.2601321150244402</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="14" t="s">
         <v>131</v>
       </c>
     </row>
@@ -8485,7 +8494,7 @@
       <c r="E20" s="6">
         <v>-0.76752428074579182</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="14" t="s">
         <v>132</v>
       </c>
     </row>
@@ -8497,7 +8506,7 @@
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="14" t="s">
         <v>133</v>
       </c>
     </row>
@@ -8514,7 +8523,7 @@
       <c r="E22" s="6">
         <v>-2.381554277909903</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="14" t="s">
         <v>134</v>
       </c>
     </row>
@@ -8531,7 +8540,7 @@
       <c r="E23" s="6">
         <v>0.16977422353168681</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="14" t="s">
         <v>135</v>
       </c>
     </row>
@@ -8548,7 +8557,7 @@
       <c r="E24" s="6">
         <v>-2.4841354129104225</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="14" t="s">
         <v>136</v>
       </c>
     </row>
@@ -8565,7 +8574,7 @@
       <c r="E25" s="6">
         <v>-2.3375668045523486</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="14" t="s">
         <v>137</v>
       </c>
     </row>
@@ -8582,7 +8591,7 @@
       <c r="E26" s="6">
         <v>-1.5570368550412756</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="14" t="s">
         <v>138</v>
       </c>
     </row>
@@ -8599,7 +8608,7 @@
       <c r="E27" s="6">
         <v>-2.9379786175002378</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="14" t="s">
         <v>139</v>
       </c>
     </row>
@@ -8616,7 +8625,7 @@
       <c r="E28" s="6">
         <v>-1.2093379424969983</v>
       </c>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="14" t="s">
         <v>140</v>
       </c>
     </row>
@@ -8633,7 +8642,7 @@
       <c r="E29" s="6">
         <v>-0.71866405148234058</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="14" t="s">
         <v>141</v>
       </c>
     </row>
@@ -8650,7 +8659,7 @@
       <c r="E30" s="6">
         <v>-0.22417847748706432</v>
       </c>
-      <c r="G30" s="15" t="s">
+      <c r="G30" s="14" t="s">
         <v>142</v>
       </c>
     </row>
@@ -8667,7 +8676,7 @@
       <c r="E31" s="6">
         <v>-0.15567976326000821</v>
       </c>
-      <c r="G31" s="15" t="s">
+      <c r="G31" s="14" t="s">
         <v>143</v>
       </c>
     </row>
@@ -8684,7 +8693,7 @@
       <c r="E32" s="6">
         <v>-0.37309147590459624</v>
       </c>
-      <c r="G32" s="15" t="s">
+      <c r="G32" s="14" t="s">
         <v>144</v>
       </c>
     </row>
@@ -8701,7 +8710,7 @@
       <c r="E33" s="6">
         <v>0.11389469349622505</v>
       </c>
-      <c r="G33" s="15" t="s">
+      <c r="G33" s="14" t="s">
         <v>145</v>
       </c>
     </row>
@@ -8718,7 +8727,7 @@
       <c r="E34" s="6">
         <v>-0.2820402294659905</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="G34" s="14" t="s">
         <v>146</v>
       </c>
     </row>
@@ -8735,7 +8744,7 @@
       <c r="E35" s="6">
         <v>-0.28247153633544286</v>
       </c>
-      <c r="G35" s="15" t="s">
+      <c r="G35" s="14" t="s">
         <v>147</v>
       </c>
     </row>
@@ -8752,7 +8761,7 @@
       <c r="E36" s="6">
         <v>-1.7467927052276622E-2</v>
       </c>
-      <c r="G36" s="15" t="s">
+      <c r="G36" s="14" t="s">
         <v>148</v>
       </c>
     </row>
@@ -8769,7 +8778,7 @@
       <c r="E37" s="6">
         <v>-1.0663526189105026</v>
       </c>
-      <c r="G37" s="15" t="s">
+      <c r="G37" s="14" t="s">
         <v>149</v>
       </c>
     </row>
@@ -8786,7 +8795,7 @@
       <c r="E38" s="6">
         <v>3.4530441518240806E-2</v>
       </c>
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="14" t="s">
         <v>150</v>
       </c>
     </row>
@@ -8803,7 +8812,7 @@
       <c r="E39" s="6">
         <v>-0.38170658178027139</v>
       </c>
-      <c r="G39" s="15" t="s">
+      <c r="G39" s="14" t="s">
         <v>151</v>
       </c>
     </row>
@@ -8820,7 +8829,7 @@
       <c r="E40" s="6">
         <v>-0.8317636741596619</v>
       </c>
-      <c r="G40" s="15" t="s">
+      <c r="G40" s="14" t="s">
         <v>152</v>
       </c>
     </row>
@@ -8837,7 +8846,7 @@
       <c r="E41" s="6">
         <v>-0.85570110914833108</v>
       </c>
-      <c r="G41" s="15" t="s">
+      <c r="G41" s="14" t="s">
         <v>153</v>
       </c>
     </row>
@@ -8854,7 +8863,7 @@
       <c r="E42" s="6">
         <v>-0.64003029860167082</v>
       </c>
-      <c r="G42" s="15" t="s">
+      <c r="G42" s="14" t="s">
         <v>154</v>
       </c>
     </row>
@@ -8871,7 +8880,7 @@
       <c r="E43" s="6">
         <v>-0.29253649877241283</v>
       </c>
-      <c r="G43" s="15" t="s">
+      <c r="G43" s="14" t="s">
         <v>155</v>
       </c>
     </row>
@@ -8888,7 +8897,7 @@
       <c r="E44" s="6">
         <v>-2.4311866921133549</v>
       </c>
-      <c r="G44" s="15" t="s">
+      <c r="G44" s="14" t="s">
         <v>156</v>
       </c>
     </row>
@@ -8905,7 +8914,7 @@
       <c r="E45" s="6">
         <v>-1.0027666204152901</v>
       </c>
-      <c r="G45" s="15" t="s">
+      <c r="G45" s="14" t="s">
         <v>157</v>
       </c>
     </row>
@@ -8922,7 +8931,7 @@
       <c r="E46" s="6">
         <v>-7.7459125560157993E-2</v>
       </c>
-      <c r="G46" s="15" t="s">
+      <c r="G46" s="14" t="s">
         <v>158</v>
       </c>
     </row>
@@ -8939,7 +8948,7 @@
       <c r="E47" s="6">
         <v>-1.0597702788743515</v>
       </c>
-      <c r="G47" s="15" t="s">
+      <c r="G47" s="14" t="s">
         <v>159</v>
       </c>
     </row>
@@ -8956,7 +8965,7 @@
       <c r="E48" s="6">
         <v>-0.9619901103319517</v>
       </c>
-      <c r="G48" s="15" t="s">
+      <c r="G48" s="14" t="s">
         <v>160</v>
       </c>
     </row>
@@ -8973,7 +8982,7 @@
       <c r="E49" s="6">
         <v>-0.49622795613140003</v>
       </c>
-      <c r="G49" s="15" t="s">
+      <c r="G49" s="14" t="s">
         <v>161</v>
       </c>
     </row>
@@ -8990,7 +8999,7 @@
       <c r="E50" s="6">
         <v>-1.3304152914216902</v>
       </c>
-      <c r="G50" s="15" t="s">
+      <c r="G50" s="14" t="s">
         <v>162</v>
       </c>
     </row>
@@ -9007,7 +9016,7 @@
       <c r="E51" s="6">
         <v>-0.81782030299491471</v>
       </c>
-      <c r="G51" s="15" t="s">
+      <c r="G51" s="14" t="s">
         <v>163</v>
       </c>
     </row>
@@ -9024,7 +9033,7 @@
       <c r="E52" s="6">
         <v>-0.52934470319236393</v>
       </c>
-      <c r="G52" s="15" t="s">
+      <c r="G52" s="14" t="s">
         <v>164</v>
       </c>
     </row>
@@ -9041,7 +9050,7 @@
       <c r="E53" s="6">
         <v>0.51671460162499905</v>
       </c>
-      <c r="G53" s="15" t="s">
+      <c r="G53" s="14" t="s">
         <v>165</v>
       </c>
     </row>
@@ -9058,7 +9067,7 @@
       <c r="E54" s="6">
         <v>-0.13411129411543143</v>
       </c>
-      <c r="G54" s="15" t="s">
+      <c r="G54" s="14" t="s">
         <v>166</v>
       </c>
     </row>
@@ -9075,7 +9084,7 @@
       <c r="E55" s="6">
         <v>-0.31425956558341106</v>
       </c>
-      <c r="G55" s="15" t="s">
+      <c r="G55" s="14" t="s">
         <v>167</v>
       </c>
     </row>
@@ -9092,7 +9101,7 @@
       <c r="E56" s="6">
         <v>-1.4493851744040676</v>
       </c>
-      <c r="G56" s="15" t="s">
+      <c r="G56" s="14" t="s">
         <v>168</v>
       </c>
     </row>
@@ -9109,7 +9118,7 @@
       <c r="E57" s="6">
         <v>-0.65231903733176466</v>
       </c>
-      <c r="G57" s="15" t="s">
+      <c r="G57" s="14" t="s">
         <v>169</v>
       </c>
     </row>
@@ -9126,7 +9135,7 @@
       <c r="E58" s="6">
         <v>-2.1163790816722896</v>
       </c>
-      <c r="G58" s="15" t="s">
+      <c r="G58" s="14" t="s">
         <v>170</v>
       </c>
     </row>
@@ -9143,7 +9152,7 @@
       <c r="E59" s="6">
         <v>-0.7117694054479653</v>
       </c>
-      <c r="G59" s="15" t="s">
+      <c r="G59" s="14" t="s">
         <v>171</v>
       </c>
     </row>
@@ -9160,7 +9169,7 @@
       <c r="E60" s="6">
         <v>-0.14578154798368725</v>
       </c>
-      <c r="G60" s="15" t="s">
+      <c r="G60" s="14" t="s">
         <v>172</v>
       </c>
     </row>
@@ -9171,7 +9180,7 @@
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
-      <c r="G61" s="15" t="s">
+      <c r="G61" s="14" t="s">
         <v>173</v>
       </c>
     </row>
@@ -9182,7 +9191,7 @@
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
       <c r="E62" s="8"/>
-      <c r="G62" s="15" t="s">
+      <c r="G62" s="14" t="s">
         <v>174</v>
       </c>
     </row>
@@ -9199,7 +9208,7 @@
       <c r="E63" s="6">
         <v>-1.2386139793506921</v>
       </c>
-      <c r="G63" s="15" t="s">
+      <c r="G63" s="14" t="s">
         <v>175</v>
       </c>
     </row>
@@ -9216,7 +9225,7 @@
       <c r="E64" s="6">
         <v>-4.9328349758112289E-2</v>
       </c>
-      <c r="G64" s="15" t="s">
+      <c r="G64" s="14" t="s">
         <v>176</v>
       </c>
     </row>
@@ -9233,7 +9242,7 @@
       <c r="E65" s="6">
         <v>-4.518718337023131E-2</v>
       </c>
-      <c r="G65" s="15" t="s">
+      <c r="G65" s="14" t="s">
         <v>177</v>
       </c>
     </row>
@@ -9250,7 +9259,7 @@
       <c r="E66" s="6">
         <v>4.9692160584632106E-2</v>
       </c>
-      <c r="G66" s="15" t="s">
+      <c r="G66" s="14" t="s">
         <v>178</v>
       </c>
     </row>
@@ -9262,7 +9271,7 @@
       <c r="D67" s="8"/>
       <c r="E67" s="8"/>
       <c r="F67" s="10"/>
-      <c r="G67" s="15" t="s">
+      <c r="G67" s="14" t="s">
         <v>179</v>
       </c>
     </row>
@@ -9279,7 +9288,7 @@
       <c r="E68" s="6">
         <v>-0.58589359506374894</v>
       </c>
-      <c r="G68" s="15" t="s">
+      <c r="G68" s="14" t="s">
         <v>180</v>
       </c>
     </row>
@@ -9290,7 +9299,7 @@
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
       <c r="E69" s="8"/>
-      <c r="G69" s="15" t="s">
+      <c r="G69" s="14" t="s">
         <v>181</v>
       </c>
     </row>
@@ -9307,7 +9316,7 @@
       <c r="E70" s="6">
         <v>-1.8346241726966102</v>
       </c>
-      <c r="G70" s="15" t="s">
+      <c r="G70" s="14" t="s">
         <v>182</v>
       </c>
     </row>
@@ -9324,7 +9333,7 @@
       <c r="E71" s="6">
         <v>-0.9731192512890976</v>
       </c>
-      <c r="G71" s="15" t="s">
+      <c r="G71" s="14" t="s">
         <v>183</v>
       </c>
     </row>
@@ -9341,7 +9350,7 @@
       <c r="E72" s="6">
         <v>-1.1803755682145809</v>
       </c>
-      <c r="G72" s="15" t="s">
+      <c r="G72" s="14" t="s">
         <v>184</v>
       </c>
     </row>
@@ -9358,7 +9367,7 @@
       <c r="E73" s="6">
         <v>-0.95611884302475136</v>
       </c>
-      <c r="G73" s="15" t="s">
+      <c r="G73" s="14" t="s">
         <v>185</v>
       </c>
     </row>
@@ -9369,7 +9378,7 @@
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
       <c r="E74" s="8"/>
-      <c r="G74" s="15" t="s">
+      <c r="G74" s="14" t="s">
         <v>186</v>
       </c>
     </row>
@@ -9386,7 +9395,7 @@
       <c r="E75" s="6">
         <v>4.008887009564166E-2</v>
       </c>
-      <c r="G75" s="15" t="s">
+      <c r="G75" s="14" t="s">
         <v>187</v>
       </c>
     </row>
@@ -9403,7 +9412,7 @@
       <c r="E76" s="6">
         <v>4.9353543474047079E-2</v>
       </c>
-      <c r="G76" s="15" t="s">
+      <c r="G76" s="14" t="s">
         <v>188</v>
       </c>
     </row>
@@ -9420,7 +9429,7 @@
       <c r="E77" s="6">
         <v>-1.6154460919688214</v>
       </c>
-      <c r="G77" s="15" t="s">
+      <c r="G77" s="14" t="s">
         <v>189</v>
       </c>
     </row>
@@ -9433,7 +9442,7 @@
       <c r="E78" s="6">
         <v>-4.9336138120977875</v>
       </c>
-      <c r="G78" s="15" t="s">
+      <c r="G78" s="14" t="s">
         <v>190</v>
       </c>
     </row>
@@ -9450,7 +9459,7 @@
       <c r="E79" s="6">
         <v>-2.4880096088241901</v>
       </c>
-      <c r="G79" s="15" t="s">
+      <c r="G79" s="14" t="s">
         <v>191</v>
       </c>
     </row>
@@ -9467,7 +9476,7 @@
       <c r="E80" s="6">
         <v>-3.0067571031480953</v>
       </c>
-      <c r="G80" s="15" t="s">
+      <c r="G80" s="14" t="s">
         <v>192</v>
       </c>
     </row>
@@ -9484,7 +9493,7 @@
       <c r="E81" s="6">
         <v>-0.27910517638973431</v>
       </c>
-      <c r="G81" s="15" t="s">
+      <c r="G81" s="14" t="s">
         <v>195</v>
       </c>
     </row>
@@ -9501,7 +9510,7 @@
       <c r="E82" s="6">
         <v>-0.18525520290728892</v>
       </c>
-      <c r="G82" s="15" t="s">
+      <c r="G82" s="14" t="s">
         <v>196</v>
       </c>
     </row>
@@ -9518,7 +9527,7 @@
       <c r="E83" s="6">
         <v>-2.6491830782532682</v>
       </c>
-      <c r="G83" s="15" t="s">
+      <c r="G83" s="14" t="s">
         <v>197</v>
       </c>
     </row>
@@ -9535,7 +9544,7 @@
       <c r="E84" s="6">
         <v>-4.1554625617141436</v>
       </c>
-      <c r="G84" s="15" t="s">
+      <c r="G84" s="14" t="s">
         <v>198</v>
       </c>
     </row>
@@ -9552,7 +9561,7 @@
       <c r="E85" s="6">
         <v>-3.6548602111449586</v>
       </c>
-      <c r="G85" s="15" t="s">
+      <c r="G85" s="14" t="s">
         <v>199</v>
       </c>
     </row>
@@ -9563,7 +9572,7 @@
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
       <c r="E86" s="8"/>
-      <c r="G86" s="15" t="s">
+      <c r="G86" s="14" t="s">
         <v>200</v>
       </c>
     </row>
@@ -9574,7 +9583,7 @@
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
       <c r="E87" s="8"/>
-      <c r="G87" s="15" t="s">
+      <c r="G87" s="14" t="s">
         <v>201</v>
       </c>
     </row>
@@ -9591,7 +9600,7 @@
       <c r="E88" s="6">
         <v>-1.740471672095012E-2</v>
       </c>
-      <c r="G88" s="15" t="s">
+      <c r="G88" s="14" t="s">
         <v>202</v>
       </c>
     </row>
@@ -9602,7 +9611,7 @@
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
       <c r="E89" s="8"/>
-      <c r="G89" s="15" t="s">
+      <c r="G89" s="14" t="s">
         <v>203</v>
       </c>
     </row>
@@ -9619,7 +9628,7 @@
       <c r="E90" s="6">
         <v>-2.6402512573863421</v>
       </c>
-      <c r="G90" s="15" t="s">
+      <c r="G90" s="14" t="s">
         <v>204</v>
       </c>
     </row>
@@ -9630,7 +9639,7 @@
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
       <c r="E91" s="8"/>
-      <c r="G91" s="15" t="s">
+      <c r="G91" s="14" t="s">
         <v>205</v>
       </c>
     </row>
@@ -9647,7 +9656,7 @@
       <c r="E92" s="6">
         <v>-2.1750803898605011</v>
       </c>
-      <c r="G92" s="15" t="s">
+      <c r="G92" s="14" t="s">
         <v>206</v>
       </c>
     </row>
@@ -9660,7 +9669,7 @@
       <c r="E93" s="6">
         <v>-4.53567380342575</v>
       </c>
-      <c r="G93" s="15" t="s">
+      <c r="G93" s="14" t="s">
         <v>207</v>
       </c>
     </row>
@@ -9677,7 +9686,7 @@
       <c r="E94" s="6">
         <v>-2.0591319943983213</v>
       </c>
-      <c r="G94" s="15" t="s">
+      <c r="G94" s="14" t="s">
         <v>208</v>
       </c>
     </row>
@@ -9694,7 +9703,7 @@
       <c r="E95" s="6">
         <v>-1.5854063354121615</v>
       </c>
-      <c r="G95" s="15" t="s">
+      <c r="G95" s="14" t="s">
         <v>209</v>
       </c>
     </row>
@@ -9705,7 +9714,7 @@
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
       <c r="E96" s="8"/>
-      <c r="G96" s="15" t="s">
+      <c r="G96" s="14" t="s">
         <v>210</v>
       </c>
     </row>
@@ -9716,7 +9725,7 @@
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
       <c r="E97" s="8"/>
-      <c r="G97" s="15" t="s">
+      <c r="G97" s="14" t="s">
         <v>211</v>
       </c>
     </row>
@@ -9727,7 +9736,7 @@
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
       <c r="E98" s="8"/>
-      <c r="G98" s="15" t="s">
+      <c r="G98" s="14" t="s">
         <v>212</v>
       </c>
     </row>
@@ -9738,7 +9747,7 @@
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
       <c r="E99" s="8"/>
-      <c r="G99" s="15" t="s">
+      <c r="G99" s="14" t="s">
         <v>214</v>
       </c>
     </row>
@@ -9755,7 +9764,7 @@
       <c r="E100" s="6">
         <v>0.22165996190507276</v>
       </c>
-      <c r="G100" s="15" t="s">
+      <c r="G100" s="14" t="s">
         <v>215</v>
       </c>
     </row>
@@ -9772,7 +9781,7 @@
       <c r="E101" s="6">
         <v>-3.3425492050712884</v>
       </c>
-      <c r="G101" s="15" t="s">
+      <c r="G101" s="14" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9789,7 +9798,7 @@
       <c r="E102" s="6">
         <v>-0.24395428411410158</v>
       </c>
-      <c r="G102" s="15" t="s">
+      <c r="G102" s="14" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9806,7 +9815,7 @@
       <c r="E103" s="6">
         <v>0</v>
       </c>
-      <c r="G103" s="15" t="s">
+      <c r="G103" s="14" t="s">
         <v>220</v>
       </c>
     </row>

</xml_diff>